<commit_message>
Finished the configuration creation pipeline
</commit_message>
<xml_diff>
--- a/Parameter Explanations.xlsx
+++ b/Parameter Explanations.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal-Study\Programming\disco-diffusion-dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Personal Study\Programming\disco-diffusion-dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3691F263-FC4A-4AE4-BDC1-01A163E2E2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-19080" yWindow="1485" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -21,16 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -604,7 +595,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -975,26 +966,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C64" sqref="C64"/>
+      <selection pane="bottomRight" activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1015625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26171875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.15625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -1020,334 +1011,265 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>72</v>
       </c>
-      <c r="B2" t="s">
+      <c r="H9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>156</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>159</v>
+      </c>
+      <c r="H13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>162</v>
+      </c>
+      <c r="H15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>162</v>
+      </c>
+      <c r="H16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" t="s">
         <v>76</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C18" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B19" t="s">
         <v>91</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>102</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" t="s">
-        <v>95</v>
       </c>
       <c r="C19" t="s">
         <v>84</v>
@@ -1355,19 +1277,16 @@
       <c r="D19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E19" t="s">
-        <v>97</v>
-      </c>
       <c r="F19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>84</v>
@@ -1375,68 +1294,62 @@
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
-        <v>98</v>
-      </c>
       <c r="F20" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" t="s">
-        <v>127</v>
+        <v>84</v>
+      </c>
+      <c r="D21" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="F21" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" t="s">
-        <v>131</v>
+        <v>84</v>
+      </c>
+      <c r="D22" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.05</v>
+        <v>84</v>
+      </c>
+      <c r="D23" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1445,906 +1358,984 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>122</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.05</v>
+        <v>84</v>
+      </c>
+      <c r="D24" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
         <v>110</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.8</v>
+        <v>84</v>
+      </c>
+      <c r="D25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>114</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="2">
-        <v>2</v>
+        <v>84</v>
+      </c>
+      <c r="D26" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>117</v>
       </c>
       <c r="F26" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1500</v>
+        <v>84</v>
+      </c>
+      <c r="D27" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="2">
-        <v>10000</v>
+        <v>84</v>
+      </c>
+      <c r="D28" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="2">
-        <v>5000</v>
+        <v>84</v>
+      </c>
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>99</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="2">
-        <v>4</v>
+        <v>84</v>
+      </c>
+      <c r="D30" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>100</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="2">
-        <v>150</v>
+        <v>84</v>
+      </c>
+      <c r="D31" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>101</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="D32" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>102</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" s="2">
-        <v>250</v>
+        <v>84</v>
+      </c>
+      <c r="D33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>103</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="D34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>96</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="2">
-        <v>50</v>
+        <v>84</v>
+      </c>
+      <c r="D35" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
-      <c r="H35" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B36" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="2">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="D36" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1</v>
+        <v>129</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="E37" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H37" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="2">
-        <v>16</v>
+        <v>129</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" t="s">
+        <v>131</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
         <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="D39" s="2">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
         <v>110</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="D40" s="2">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>111</v>
+        <v>0.05</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
-      <c r="H40" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="D41" s="2">
-        <v>1000</v>
+        <v>0.8</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
         <v>80</v>
       </c>
       <c r="D42" s="2">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
       </c>
       <c r="C43" t="s">
         <v>80</v>
       </c>
       <c r="D43" s="2">
-        <v>0</v>
-      </c>
-      <c r="E43" t="s">
-        <v>157</v>
+        <v>1500</v>
       </c>
       <c r="F43" t="b">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
         <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
-      </c>
-      <c r="D44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="2">
+        <v>5000</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="2">
+        <v>4</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="2">
         <v>150</v>
       </c>
-      <c r="E44" t="s">
-        <v>151</v>
-      </c>
-      <c r="F44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" t="s">
-        <v>79</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E47" t="s">
-        <v>92</v>
-      </c>
       <c r="F47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="E48" t="s">
-        <v>107</v>
+        <v>80</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>106</v>
+        <v>80</v>
+      </c>
+      <c r="D49" s="2">
+        <v>250</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E50" t="s">
-        <v>94</v>
+        <v>80</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="B51" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>79</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>105</v>
+        <v>80</v>
+      </c>
+      <c r="D51" s="2">
+        <v>50</v>
+      </c>
+      <c r="E51" t="s">
+        <v>133</v>
       </c>
       <c r="F51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H51" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B52" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>79</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>164</v>
+        <v>80</v>
+      </c>
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>135</v>
       </c>
       <c r="F52" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
-        <v>79</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>125</v>
+        <v>80</v>
+      </c>
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>137</v>
       </c>
       <c r="F53" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
         <v>110</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>124</v>
+        <v>80</v>
+      </c>
+      <c r="D54" s="2">
+        <v>16</v>
       </c>
       <c r="F54" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
         <v>110</v>
       </c>
       <c r="C55" t="s">
-        <v>79</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>123</v>
+        <v>80</v>
+      </c>
+      <c r="D55" s="2">
+        <v>1</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
         <v>110</v>
       </c>
       <c r="C56" t="s">
-        <v>79</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>118</v>
+        <v>80</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="H56" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E57" t="s">
-        <v>121</v>
+        <v>80</v>
+      </c>
+      <c r="D57" s="2">
+        <v>1000</v>
       </c>
       <c r="F57" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>79</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B59" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C59" t="s">
         <v>79</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E59" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>57</v>
+      </c>
+      <c r="B60" t="s">
+        <v>91</v>
       </c>
       <c r="C60" t="s">
         <v>79</v>
       </c>
+      <c r="D60" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="F60" t="b">
-        <v>1</v>
-      </c>
-      <c r="G60" t="s">
-        <v>51</v>
-      </c>
-      <c r="H60" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>91</v>
+      </c>
+      <c r="C61" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E62" t="s">
+        <v>92</v>
+      </c>
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>107</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>55</v>
+      </c>
+      <c r="B64" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" t="s">
+        <v>79</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" t="s">
+        <v>94</v>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" t="s">
+        <v>91</v>
+      </c>
+      <c r="C66" t="s">
+        <v>79</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" t="s">
+        <v>79</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" t="s">
+        <v>110</v>
+      </c>
+      <c r="C71" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E71" t="s">
+        <v>119</v>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>52</v>
+      </c>
+      <c r="B72" t="s">
+        <v>110</v>
+      </c>
+      <c r="C72" t="s">
+        <v>79</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" t="s">
+        <v>121</v>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>54</v>
+      </c>
+      <c r="B73" t="s">
+        <v>110</v>
+      </c>
+      <c r="C73" t="s">
+        <v>79</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E73" t="s">
+        <v>116</v>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" t="s">
+        <v>79</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" t="s">
+        <v>144</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>26</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B75" t="s">
         <v>85</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C75" t="s">
         <v>87</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E75" t="s">
         <v>89</v>
       </c>
-      <c r="F61" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
-        <v>1</v>
-      </c>
-      <c r="F62" t="b">
-        <v>1</v>
-      </c>
-      <c r="G62" t="s">
-        <v>0</v>
-      </c>
-      <c r="H62" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" t="b">
-        <v>1</v>
-      </c>
-      <c r="H63" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" t="b">
-        <v>1</v>
-      </c>
-      <c r="G64" t="s">
-        <v>138</v>
-      </c>
-      <c r="H64" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" t="b">
-        <v>1</v>
-      </c>
-      <c r="G65" t="s">
-        <v>51</v>
-      </c>
-      <c r="H65" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" t="s">
-        <v>30</v>
-      </c>
-      <c r="F66" t="b">
-        <v>1</v>
-      </c>
-      <c r="G66" t="s">
-        <v>147</v>
-      </c>
-      <c r="H66" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" t="s">
-        <v>46</v>
-      </c>
-      <c r="F67" t="b">
-        <v>1</v>
-      </c>
-      <c r="G67" t="s">
-        <v>149</v>
-      </c>
-      <c r="H67" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" t="s">
-        <v>48</v>
-      </c>
-      <c r="F68" t="b">
-        <v>1</v>
-      </c>
-      <c r="G68" t="s">
-        <v>52</v>
-      </c>
-      <c r="H68" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" t="s">
-        <v>56</v>
-      </c>
-      <c r="E69" t="s">
-        <v>155</v>
-      </c>
-      <c r="F69" t="b">
-        <v>1</v>
-      </c>
-      <c r="G69" t="s">
-        <v>72</v>
-      </c>
-      <c r="H69" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" t="s">
-        <v>58</v>
-      </c>
-      <c r="E70" t="s">
-        <v>156</v>
-      </c>
-      <c r="F70" t="b">
-        <v>1</v>
-      </c>
-      <c r="G70" t="s">
-        <v>72</v>
-      </c>
-      <c r="H70" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" t="s">
-        <v>61</v>
-      </c>
-      <c r="F71" t="b">
-        <v>1</v>
-      </c>
-      <c r="G71" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" t="s">
-        <v>67</v>
-      </c>
-      <c r="F72" t="b">
-        <v>1</v>
-      </c>
-      <c r="G72" t="s">
-        <v>159</v>
-      </c>
-      <c r="H72" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" t="s">
-        <v>71</v>
-      </c>
-      <c r="F73" t="b">
-        <v>1</v>
-      </c>
-      <c r="G73" t="s">
-        <v>162</v>
-      </c>
-      <c r="H73" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" t="s">
-        <v>73</v>
-      </c>
-      <c r="F74" t="b">
-        <v>1</v>
-      </c>
-      <c r="G74" t="s">
-        <v>68</v>
-      </c>
-      <c r="H74" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" t="s">
-        <v>70</v>
-      </c>
       <c r="F75" t="b">
-        <v>1</v>
-      </c>
-      <c r="G75" t="s">
-        <v>162</v>
-      </c>
-      <c r="H75" t="s">
-        <v>163</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H75">
-    <sortState ref="A2:H75">
-      <sortCondition ref="C1:C75"/>
+  <autoFilter ref="A1:H75" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
+      <sortCondition ref="A1:A75"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:H75">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H75">
     <sortCondition ref="B1:B75"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added deletion of config files after jobs are run
</commit_message>
<xml_diff>
--- a/Parameter Explanations.xlsx
+++ b/Parameter Explanations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Personal Study\Programming\disco-diffusion-dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098F59B7-62D7-4F64-9D81-2D6DAA87E1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEFF82D-7B21-44E1-9A80-66BECFCEC073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="2535" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28095" yWindow="495" windowWidth="27945" windowHeight="13455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -597,7 +597,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated init skip steps slider
</commit_message>
<xml_diff>
--- a/Parameter Explanations.xlsx
+++ b/Parameter Explanations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Personal Study\Programming\disco-diffusion-dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEFF82D-7B21-44E1-9A80-66BECFCEC073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A30A1D8-9DBC-4004-ADDB-916268A21D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28095" yWindow="495" windowWidth="27945" windowHeight="13455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="18000" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="73">
   <si>
     <t>batch_name</t>
   </si>
@@ -220,6 +220,33 @@
   </si>
   <si>
     <t xml:space="preserve">How many steps you'll skip; diffusion has a higher learning rate on earlier steps, so for init images, higher values will result in an image closer to the original image. Defaults to 0 without an init image, and 140 with one. </t>
+  </si>
+  <si>
+    <t>create_mp4</t>
+  </si>
+  <si>
+    <t>Video Generation</t>
+  </si>
+  <si>
+    <t>mp4_fps</t>
+  </si>
+  <si>
+    <t>Video FPS</t>
+  </si>
+  <si>
+    <t>save_all_images</t>
+  </si>
+  <si>
+    <t>Intermediate Images</t>
+  </si>
+  <si>
+    <t>Whether or not to save image files for all of the diffusion steps, or just the final ones. If unchecked, intermediate images will delete once diffusion is complete.</t>
+  </si>
+  <si>
+    <t>Whether or not you want to save a video showing the start-to-finish diffusion process.</t>
+  </si>
+  <si>
+    <t>How many frames per second the video is.</t>
   </si>
 </sst>
 </file>
@@ -594,10 +621,10 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +715,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="3">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>41</v>
@@ -981,6 +1008,57 @@
       </c>
       <c r="E22" s="3" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="3">
+        <v>30</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>